<commit_message>
Aggiunta codice rischio provinciale
</commit_message>
<xml_diff>
--- a/R/data/abitanti_istat.xlsx
+++ b/R/data/abitanti_istat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzonardelli/Dropbox/projects/covid/codici/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigigiuseppeatzeni/Dropbox/codici/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F47D20D-B524-6E46-B1D9-BB97E3B82788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BCAA14-B8F4-9E47-B6DF-672753E18953}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>Rimini</t>
   </si>
   <si>
-    <t>Massa-Carrara</t>
-  </si>
-  <si>
     <t>Lucca</t>
   </si>
   <si>
@@ -347,23 +344,26 @@
     <t>Sud Sardegna</t>
   </si>
   <si>
-    <t>prov_name</t>
-  </si>
-  <si>
     <t>abitanti</t>
   </si>
   <si>
-    <t>Bolzano/Bozen</t>
-  </si>
-  <si>
-    <t>Valle d'Aosta/Vallée d'Aoste</t>
+    <t>Aosta</t>
+  </si>
+  <si>
+    <t>Provincia</t>
+  </si>
+  <si>
+    <t>Massa Carrara</t>
+  </si>
+  <si>
+    <t>Bolzano</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -494,12 +494,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lucida Grande"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -848,10 +842,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1209,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1219,11 +1212,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>105</v>
+      <c r="A1" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -1290,9 +1283,9 @@
         <v>158349</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B10">
         <v>125666</v>
@@ -1427,8 +1420,8 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
-        <v>107</v>
+      <c r="A27" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="B27">
         <v>531178</v>
@@ -1603,8 +1596,8 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
-        <v>45</v>
+      <c r="A49" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="B49">
         <v>194878</v>
@@ -1612,7 +1605,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50">
         <v>387876</v>
@@ -1620,7 +1613,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51">
         <v>292473</v>
@@ -1628,7 +1621,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52">
         <v>1011349</v>
@@ -1636,7 +1629,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53">
         <v>334832</v>
@@ -1644,7 +1637,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54">
         <v>419037</v>
@@ -1652,7 +1645,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55">
         <v>342654</v>
@@ -1660,7 +1653,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56">
         <v>267197</v>
@@ -1668,7 +1661,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57">
         <v>221629</v>
@@ -1676,7 +1669,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58">
         <v>257716</v>
@@ -1684,7 +1677,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B59">
         <v>656382</v>
@@ -1692,7 +1685,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B60">
         <v>225633</v>
@@ -1700,7 +1693,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B61">
         <v>358886</v>
@@ -1708,7 +1701,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B62">
         <v>471228</v>
@@ -1716,7 +1709,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B63">
         <v>314178</v>
@@ -1724,7 +1717,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B64">
         <v>207179</v>
@@ -1732,7 +1725,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B65">
         <v>173800</v>
@@ -1740,7 +1733,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B66">
         <v>317030</v>
@@ -1748,7 +1741,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B67">
         <v>155503</v>
@@ -1756,7 +1749,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B68">
         <v>4342212</v>
@@ -1764,7 +1757,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B69">
         <v>575254</v>
@@ -1772,7 +1765,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B70">
         <v>489083</v>
@@ -1780,7 +1773,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B71">
         <v>299031</v>
@@ -1788,7 +1781,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B72">
         <v>308052</v>
@@ -1796,7 +1789,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B73">
         <v>318909</v>
@@ -1804,7 +1797,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B74">
         <v>385588</v>
@@ -1812,7 +1805,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B75">
         <v>221238</v>
@@ -1820,7 +1813,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B76">
         <v>84379</v>
@@ -1828,7 +1821,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B77">
         <v>922965</v>
@@ -1836,7 +1829,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B78">
         <v>277018</v>
@@ -1844,7 +1837,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B79">
         <v>3084890</v>
@@ -1852,7 +1845,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B80">
         <v>418306</v>
@@ -1860,7 +1853,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B81">
         <v>1098513</v>
@@ -1868,7 +1861,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B82">
         <v>622183</v>
@@ -1876,7 +1869,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B83">
         <v>1251994</v>
@@ -1884,7 +1877,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B84">
         <v>576756</v>
@@ -1892,7 +1885,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B85">
         <v>392975</v>
@@ -1900,7 +1893,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B86">
         <v>795134</v>
@@ -1908,7 +1901,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B87">
         <v>390011</v>
@@ -1916,7 +1909,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B88">
         <v>364960</v>
@@ -1924,7 +1917,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B89">
         <v>197909</v>
@@ -1932,7 +1925,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B90">
         <v>705753</v>
@@ -1940,7 +1933,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B91">
         <v>358316</v>
@@ -1948,7 +1941,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B92">
         <v>548009</v>
@@ -1956,7 +1949,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B93">
         <v>174980</v>
@@ -1964,7 +1957,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B94">
         <v>160073</v>
@@ -1972,7 +1965,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B95">
         <v>430492</v>
@@ -1980,7 +1973,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96">
         <v>1252588</v>
@@ -1988,7 +1981,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B97">
         <v>626876</v>
@@ -1996,7 +1989,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B98">
         <v>434870</v>
@@ -2004,7 +1997,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B99">
         <v>262458</v>
@@ -2012,7 +2005,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B100">
         <v>164788</v>
@@ -2020,7 +2013,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B101">
         <v>1107702</v>
@@ -2028,7 +2021,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B102">
         <v>320893</v>
@@ -2036,7 +2029,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B103">
         <v>399224</v>
@@ -2044,7 +2037,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B104">
         <v>491571</v>
@@ -2052,7 +2045,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B105">
         <v>208550</v>
@@ -2060,7 +2053,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B106">
         <v>431038</v>
@@ -2068,7 +2061,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B107">
         <v>157707</v>
@@ -2076,7 +2069,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B108">
         <v>350725</v>

</xml_diff>